<commit_message>
got 74% accuracy all emotions replicated
</commit_message>
<xml_diff>
--- a/facerecognizercomparison.xlsx
+++ b/facerecognizercomparison.xlsx
@@ -25,10 +25,10 @@
     <t xml:space="preserve">Trial Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Fishfaces</t>
+    <t xml:space="preserve">LBHP</t>
   </si>
   <si>
-    <t xml:space="preserve">LBHP</t>
+    <t xml:space="preserve">Fishfaces</t>
   </si>
 </sst>
 </file>
@@ -38,7 +38,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -60,6 +60,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,7 +128,573 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LBHP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>53.59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56.46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54.07</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54.07</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55.02</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>55.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>54.55</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>54.55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53.59</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>54.07</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>55.98</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>55.98</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>48.33</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>58.85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>53.59</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50.72</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>50.72</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>51.67</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>55.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>53.11</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>53.11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>54.07</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>57.42</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>55.98</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>57.42</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>55.02</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>51.2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>55.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fishfaces</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>63.64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61.72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62.68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63.64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65.07</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66.51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>58.37</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64.11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>66.03</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64.59</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>61.24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>61.72</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>63.16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>63.64</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>55.98</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>67.46</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>64.11</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>64.59</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>62.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>65.07</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>60.29</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>64.59</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>65.07</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>64.59</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>66.51</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>65.07</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>67.46</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>60.29</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>65.55</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>65.07</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="71017605"/>
+        <c:axId val="34061525"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="71017605"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-GB" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-GB" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Trial Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="en-GB" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="34061525"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="34061525"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-GB" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-GB" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Percentage Accuracy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="en-GB" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="71017605"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" lang="en-GB" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209160</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>111240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>511200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>20880</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="2634840" y="636840"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -126,15 +702,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -476,6 +1052,26 @@
       </c>
       <c r="C31" s="0" t="n">
         <v>65.07</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="n">
+        <f aca="false">STDEV(B2:B31)</f>
+        <v>2.27654961749564</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <f aca="false">STDEV(C2:C31)</f>
+        <v>2.58993134422828</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="n">
+        <f aca="false">AVERAGE(B2:B31)</f>
+        <v>54.1633333333333</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <f aca="false">AVERAGE(C2:C31)</f>
+        <v>63.6673333333333</v>
       </c>
     </row>
   </sheetData>
@@ -486,5 +1082,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>